<commit_message>
Changed Inband EPG to Default
</commit_message>
<xml_diff>
--- a/aci-tenant-deploy_input_Spreadsheet.xlsx
+++ b/aci-tenant-deploy_input_Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1373259B-9740-4F79-B496-8E0DCB377EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58850F1-6F0A-47F3-83CB-A779F2C21B68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
   <si>
     <t>Type</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>vrf_add</t>
-  </si>
-  <si>
-    <t>tnt_add</t>
   </si>
   <si>
     <t>Prod_vrf description</t>
@@ -1468,7 +1465,7 @@
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,7 +1509,7 @@
     <row r="2" spans="1:13" s="6" customFormat="1" ht="122.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -1544,7 +1541,7 @@
       <c r="G3" s="21"/>
       <c r="H3" s="22"/>
       <c r="I3" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -1564,12 +1561,12 @@
       <c r="D4" s="14"/>
       <c r="E4" s="15"/>
       <c r="F4" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
       <c r="I4" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -1578,7 +1575,7 @@
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>39</v>
@@ -1592,7 +1589,7 @@
       <c r="G5" s="17"/>
       <c r="H5" s="18"/>
       <c r="I5" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
@@ -1988,7 +1985,7 @@
     <row r="2" spans="1:13" s="6" customFormat="1" ht="123" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2018,7 +2015,7 @@
       <c r="E3" s="25"/>
       <c r="F3" s="26"/>
       <c r="G3" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -2043,7 +2040,7 @@
       <c r="E4" s="28"/>
       <c r="F4" s="29"/>
       <c r="G4" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -2068,7 +2065,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="18"/>
       <c r="G5" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -2434,7 +2431,7 @@
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2453,19 +2450,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="F3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2477,7 +2474,7 @@
     </row>
     <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>44</v>
@@ -2486,7 +2483,7 @@
         <v>32</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
@@ -2676,7 +2673,7 @@
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2701,10 +2698,10 @@
         <v>41</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>4</v>
@@ -2915,7 +2912,7 @@
     <row r="2" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -3150,7 +3147,7 @@
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -3175,10 +3172,10 @@
         <v>41</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>4</v>
@@ -3389,7 +3386,7 @@
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -3414,10 +3411,10 @@
         <v>41</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>4</v>
@@ -3628,7 +3625,7 @@
     <row r="2" spans="1:13" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -3653,10 +3650,10 @@
         <v>41</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="F3" s="20" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
renaming python script to simply.  delete old file
</commit_message>
<xml_diff>
--- a/aci-tenant-deploy_input_Spreadsheet.xlsx
+++ b/aci-tenant-deploy_input_Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\tyscott\terraform-aci-fabric-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58850F1-6F0A-47F3-83CB-A779F2C21B68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62819FF-D2A7-4CE9-8923-881A39326D81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tenant" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
   <si>
     <t>Type</t>
   </si>
@@ -274,12 +274,6 @@
     <t>L3Out Hosting Tenant</t>
   </si>
   <si>
-    <t>L3 Domain</t>
-  </si>
-  <si>
-    <t>Routing Protocol</t>
-  </si>
-  <si>
     <t>l3out_L3</t>
   </si>
   <si>
@@ -315,6 +309,51 @@
       </rPr>
       <t>By default All VRF's are configured for enforcement; aka a Whitelist Model.  When deploying ACI for a basic network centric approach, (a typical network migration), it is best to use Preferred Group Membership or vzAny until you are ready for contract enforcement (Something that typically takes customers time to digest).  Preferred Groups is the easier way but it has a limit currently of 500 EPG's when associated to MSO.  vzAny has the larger scale but you need to implement contracts.  For this sake of this script when using vzAny, we will implement a "permit ip any any" schema but it can always be modified.  We recommend for deployments of less than 500 use preferred group.  For anything higher use vzAny.  There is not typically a reason to turn off enforcement at the VRF Level so the script doesn't expose this option.</t>
     </r>
+  </si>
+  <si>
+    <t>bgp</t>
+  </si>
+  <si>
+    <t>Create L3Outs</t>
+  </si>
+  <si>
+    <t>Leaf Name</t>
+  </si>
+  <si>
+    <t>Leaf Node Id</t>
+  </si>
+  <si>
+    <t>L3Out VRF</t>
+  </si>
+  <si>
+    <t>L3Out L3 Domain</t>
+  </si>
+  <si>
+    <t>Create Node Profiles</t>
+  </si>
+  <si>
+    <t>nodeprof</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>VLAN</t>
+  </si>
+  <si>
+    <t>IPv4/Prefix</t>
+  </si>
+  <si>
+    <t>leaf201</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>Routed Interface</t>
+  </si>
+  <si>
+    <t>1/1</t>
   </si>
 </sst>
 </file>
@@ -1464,7 +1503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1509,7 +1548,7 @@
     <row r="2" spans="1:13" s="6" customFormat="1" ht="122.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -2384,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E4AED6B-7A77-4EE3-A7F6-CBCCC2B036C0}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,7 +2452,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -2456,13 +2495,13 @@
         <v>57</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -2483,9 +2522,11 @@
         <v>32</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -2600,27 +2641,223 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
+    <row r="13" spans="1:13" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="1:13" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12"/>
+      <c r="B14" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+    </row>
+    <row r="15" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+    </row>
+    <row r="17" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+    </row>
+    <row r="21" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="B2:M2"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="B14:M14"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A5:A11" xr:uid="{281E670E-B207-4BB4-BBCC-05BA1D9AF843}">
-      <formula1>"vpc_pair"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B5 B7 B9:B11" xr:uid="{C3EB20EA-35B4-4F70-B475-957CE83E2D85}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="VPC ID" error="The VPC ID must be a number between 1 and 1000" sqref="B5 B7 B9:B11 B17 B19 B21:B23" xr:uid="{C3EB20EA-35B4-4F70-B475-957CE83E2D85}">
       <formula1>1</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4" xr:uid="{475F90AA-66B6-48D7-AE54-C9ED16DD30F9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A11" xr:uid="{475F90AA-66B6-48D7-AE54-C9ED16DD30F9}">
       <formula1>"l3out"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{649BA03F-BE92-4539-8C36-7EF4AD7D012B}">
-      <formula1>"bgp,ospf"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A16:A23" xr:uid="{206B40BC-DD10-4140-AB45-8E7BEA2CDA34}">
+      <formula1>"nodeprof"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D16" xr:uid="{83FBEA79-5C12-4771-BCC2-9B9CEBF3BDA7}">
+      <formula1>"Routed Interface,sub-interface,svi"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>